<commit_message>
added row reader and tests for that.
</commit_message>
<xml_diff>
--- a/src/test/resources/words_list.xlsx
+++ b/src/test/resources/words_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Word</t>
   </si>
@@ -46,151 +46,7 @@
     <t xml:space="preserve">усиливать</t>
   </si>
   <si>
-    <t xml:space="preserve">increase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">увеличивать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reduce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">уменьшать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drive down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">снизить</t>
-  </si>
-  <si>
-    <t xml:space="preserve">impress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">произвести впечатление</t>
-  </si>
-  <si>
-    <t xml:space="preserve">frequently</t>
-  </si>
-  <si>
-    <t xml:space="preserve">часто</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">правильный</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complexity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">сложность</t>
-  </si>
-  <si>
-    <t xml:space="preserve">force</t>
-  </si>
-  <si>
-    <t xml:space="preserve">сила</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enforce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">принуждать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">рассматривать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">considered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">считается</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">масштаб</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maintain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">поддерживать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">способность</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">частота</t>
-  </si>
-  <si>
-    <t xml:space="preserve">advantage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">преимущество</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eliminate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ликвидировать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estimation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">оценка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">essential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">существенно</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">происходить</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">иметь тенденцию</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">согласие</t>
-  </si>
-  <si>
-    <t xml:space="preserve">according</t>
-  </si>
-  <si>
-    <t xml:space="preserve">согласно</t>
-  </si>
-  <si>
-    <t xml:space="preserve">properly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">правильно</t>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -315,10 +171,10 @@
   <dimension ref="A1:B434"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.11"/>
@@ -360,202 +216,31 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
+    <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added WordTestCreator.removeValuesFromEachRowRandomCell and tests
</commit_message>
<xml_diff>
--- a/src/test/resources/words_list.xlsx
+++ b/src/test/resources/words_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="8">
   <si>
     <t xml:space="preserve">Word</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">усиливать</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -170,11 +167,11 @@
   </sheetPr>
   <dimension ref="A1:B434"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.11"/>
@@ -214,29 +211,172 @@
     </row>
     <row r="5" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>